<commit_message>
add special TR after regular ones
</commit_message>
<xml_diff>
--- a/SSR/SSR-test.xlsx
+++ b/SSR/SSR-test.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bo/Documents/projects/DomainModelExtractor/SSR/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D20D8ABC-724C-9F47-80B0-38481F559F73}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1A73C62-25E9-D746-BF8E-BA369F9B5F4F}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="23100" windowHeight="17540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="108">
   <si>
     <t>Rule</t>
   </si>
@@ -514,9 +514,6 @@
     </r>
   </si>
   <si>
-    <t>nsubj(A,B), obl*(A,C)</t>
-  </si>
-  <si>
     <t>Sentence Example</t>
   </si>
   <si>
@@ -545,9 +542,6 @@
   </si>
   <si>
     <t>SVObj</t>
-  </si>
-  <si>
-    <t>SVObl</t>
   </si>
   <si>
     <t>SVCcO</t>
@@ -834,9 +828,6 @@
     <t>12</t>
   </si>
   <si>
-    <t>1, 2, 3, 4, 5, 6, 10, 11, 12, 13</t>
-  </si>
-  <si>
     <t>Subject-Verb-By-Verb-Object</t>
   </si>
   <si>
@@ -947,6 +938,228 @@
   </si>
   <si>
     <t>SSR14</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">As a </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>seller</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">, I can replace, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>buy</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> and </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>sell</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> phones.</t>
+    </r>
+  </si>
+  <si>
+    <t>SSR15</t>
+  </si>
+  <si>
+    <t>nsubj(A,B), conj*(A,C), obj(A,D)</t>
+  </si>
+  <si>
+    <t>SSR16</t>
+  </si>
+  <si>
+    <t>Subject-Verb-CC-Verb-Object</t>
+  </si>
+  <si>
+    <t>Noun-ClausalModifier</t>
+  </si>
+  <si>
+    <t>AO</t>
+  </si>
+  <si>
+    <t>acl(A,B), obj(B,C)</t>
+  </si>
+  <si>
+    <t>A==NN*, B==VBG, C==NN*</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">As a GM, I can make </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>decision</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>affecting</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>results</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>.</t>
+    </r>
+  </si>
+  <si>
+    <t>nsubj(A,B), obl:on(A,C)</t>
+  </si>
+  <si>
+    <t>SVOblIn</t>
+  </si>
+  <si>
+    <t>SVOblOn</t>
+  </si>
+  <si>
+    <t>nsubj(A,B), obl:in(A,C)</t>
+  </si>
+  <si>
+    <t>SSR17</t>
+  </si>
+  <si>
+    <t>1, 2, 3, 4, 5, 6, 7, 11, 12, 13, 14, 15, 16</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">As a </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>student</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">, I </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>work</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> in an </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>university</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>.</t>
+    </r>
+  </si>
+  <si>
+    <t>SVCVO</t>
   </si>
 </sst>
 </file>
@@ -1853,13 +2066,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z1001"/>
+  <dimension ref="A1:Z1002"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="F3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A15" sqref="A15"/>
+      <selection pane="bottomRight" activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1893,10 +2106,10 @@
         <v>14</v>
       </c>
       <c r="G1" s="9" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="I1" s="1"/>
       <c r="J1" s="1"/>
@@ -1922,7 +2135,7 @@
         <v>4</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>18</v>
@@ -1931,7 +2144,7 @@
         <v>17</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F2" s="1"/>
       <c r="G2" s="9" t="s">
@@ -1964,16 +2177,16 @@
         <v>5</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>53</v>
+        <v>102</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>25</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>42</v>
+        <v>100</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F3" s="1"/>
       <c r="G3" s="9"/>
@@ -1999,26 +2212,26 @@
       <c r="Y3" s="1"/>
       <c r="Z3" s="1"/>
     </row>
-    <row r="4" spans="1:26" s="6" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="1" t="s">
+    <row r="4" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A4" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>54</v>
+        <v>101</v>
       </c>
-      <c r="C4" s="1" t="s">
-        <v>30</v>
+      <c r="C4" s="2" t="s">
+        <v>25</v>
       </c>
-      <c r="D4" s="3" t="s">
-        <v>22</v>
+      <c r="D4" s="2" t="s">
+        <v>103</v>
       </c>
-      <c r="E4" s="1" t="s">
-        <v>50</v>
+      <c r="E4" s="2" t="s">
+        <v>48</v>
       </c>
       <c r="F4" s="1"/>
       <c r="G4" s="9"/>
       <c r="H4" s="1" t="s">
-        <v>36</v>
+        <v>106</v>
       </c>
       <c r="I4" s="1"/>
       <c r="J4" s="1"/>
@@ -2039,28 +2252,26 @@
       <c r="Y4" s="1"/>
       <c r="Z4" s="1"/>
     </row>
-    <row r="5" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A5" s="1" t="s">
+    <row r="5" spans="1:26" s="6" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="1" t="s">
-        <v>55</v>
+      <c r="B5" s="2" t="s">
+        <v>52</v>
       </c>
-      <c r="C5" s="2" t="s">
-        <v>24</v>
+      <c r="C5" s="1" t="s">
+        <v>30</v>
       </c>
-      <c r="D5" s="2" t="s">
-        <v>16</v>
+      <c r="D5" s="3" t="s">
+        <v>22</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="F5" s="1"/>
-      <c r="G5" s="9">
-        <v>3</v>
-      </c>
+      <c r="G5" s="9"/>
       <c r="H5" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="I5" s="1"/>
       <c r="J5" s="1"/>
@@ -2082,25 +2293,27 @@
       <c r="Z5" s="1"/>
     </row>
     <row r="6" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A6" s="1" t="s">
+      <c r="A6" s="2" t="s">
         <v>8</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
-      <c r="D6" s="3" t="s">
-        <v>45</v>
+      <c r="D6" s="2" t="s">
+        <v>16</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="F6" s="1"/>
-      <c r="G6" s="9"/>
+      <c r="G6" s="9">
+        <v>3</v>
+      </c>
       <c r="H6" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="I6" s="1"/>
       <c r="J6" s="1"/>
@@ -2122,27 +2335,25 @@
       <c r="Z6" s="1"/>
     </row>
     <row r="7" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A7" s="1" t="s">
+      <c r="A7" s="2" t="s">
         <v>9</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="D7" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="E7" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="E7" s="1" t="s">
-        <v>48</v>
-      </c>
       <c r="F7" s="1"/>
-      <c r="G7" s="9" t="s">
-        <v>32</v>
-      </c>
+      <c r="G7" s="9"/>
       <c r="H7" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="I7" s="1"/>
       <c r="J7" s="1"/>
@@ -2164,27 +2375,27 @@
       <c r="Z7" s="1"/>
     </row>
     <row r="8" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A8" s="1" t="s">
+      <c r="A8" s="2" t="s">
         <v>10</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>19</v>
+        <v>55</v>
       </c>
-      <c r="C8" s="1" t="s">
-        <v>20</v>
+      <c r="C8" s="2" t="s">
+        <v>29</v>
       </c>
-      <c r="D8" s="1" t="s">
-        <v>21</v>
+      <c r="D8" s="3" t="s">
+        <v>45</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>23</v>
+        <v>47</v>
       </c>
       <c r="F8" s="1"/>
       <c r="G8" s="9" t="s">
-        <v>86</v>
+        <v>32</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="I8" s="1"/>
       <c r="J8" s="1"/>
@@ -2206,25 +2417,27 @@
       <c r="Z8" s="1"/>
     </row>
     <row r="9" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A9" s="1" t="s">
+      <c r="A9" s="2" t="s">
         <v>11</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>58</v>
+        <v>19</v>
       </c>
-      <c r="C9" s="2" t="s">
-        <v>28</v>
+      <c r="C9" s="1" t="s">
+        <v>20</v>
       </c>
-      <c r="D9" s="3" t="s">
-        <v>26</v>
+      <c r="D9" s="1" t="s">
+        <v>21</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="F9" s="1"/>
-      <c r="G9" s="9"/>
+      <c r="G9" s="9" t="s">
+        <v>105</v>
+      </c>
       <c r="H9" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="I9" s="1"/>
       <c r="J9" s="1"/>
@@ -2246,25 +2459,25 @@
       <c r="Z9" s="1"/>
     </row>
     <row r="10" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A10" s="1" t="s">
+      <c r="A10" s="2" t="s">
         <v>12</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>61</v>
+        <v>28</v>
       </c>
-      <c r="D10" s="2" t="s">
-        <v>59</v>
+      <c r="D10" s="3" t="s">
+        <v>26</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>60</v>
+        <v>27</v>
       </c>
       <c r="F10" s="1"/>
       <c r="G10" s="9"/>
       <c r="H10" s="1" t="s">
-        <v>63</v>
+        <v>41</v>
       </c>
       <c r="I10" s="1"/>
       <c r="J10" s="1"/>
@@ -2286,25 +2499,25 @@
       <c r="Z10" s="1"/>
     </row>
     <row r="11" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A11" s="1" t="s">
+      <c r="A11" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B11" s="2" t="s">
-        <v>66</v>
+      <c r="B11" s="1" t="s">
+        <v>60</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
-      <c r="D11" s="3" t="s">
-        <v>67</v>
+      <c r="D11" s="2" t="s">
+        <v>57</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>51</v>
+        <v>58</v>
       </c>
       <c r="F11" s="1"/>
       <c r="G11" s="9"/>
       <c r="H11" s="1" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="I11" s="1"/>
       <c r="J11" s="1"/>
@@ -2326,25 +2539,25 @@
       <c r="Z11" s="1"/>
     </row>
     <row r="12" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A12" s="5" t="s">
-        <v>73</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="D12" s="1" t="s">
+      <c r="A12" s="2" t="s">
         <v>71</v>
       </c>
+      <c r="B12" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>65</v>
+      </c>
       <c r="E12" s="1" t="s">
-        <v>72</v>
+        <v>50</v>
       </c>
       <c r="F12" s="1"/>
       <c r="G12" s="9"/>
       <c r="H12" s="1" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
       <c r="I12" s="1"/>
       <c r="J12" s="1"/>
@@ -2365,68 +2578,68 @@
       <c r="Y12" s="1"/>
       <c r="Z12" s="1"/>
     </row>
-    <row r="13" spans="1:26" s="6" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="5" t="s">
-        <v>79</v>
+    <row r="13" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A13" s="2" t="s">
+        <v>77</v>
       </c>
-      <c r="B13" s="2" t="s">
+      <c r="B13" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="F13" s="1"/>
+      <c r="G13" s="9"/>
+      <c r="H13" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="I13" s="1"/>
+      <c r="J13" s="1"/>
+      <c r="K13" s="1"/>
+      <c r="L13" s="1"/>
+      <c r="M13" s="1"/>
+      <c r="N13" s="1"/>
+      <c r="O13" s="1"/>
+      <c r="P13" s="1"/>
+      <c r="Q13" s="1"/>
+      <c r="R13" s="1"/>
+      <c r="S13" s="1"/>
+      <c r="T13" s="1"/>
+      <c r="U13" s="1"/>
+      <c r="V13" s="1"/>
+      <c r="W13" s="1"/>
+      <c r="X13" s="1"/>
+      <c r="Y13" s="1"/>
+      <c r="Z13" s="1"/>
+    </row>
+    <row r="14" spans="1:26" s="6" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="D14" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="C13" s="2" t="s">
+      <c r="E14" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="F14" s="5"/>
+      <c r="G14" s="10" t="s">
         <v>75</v>
       </c>
-      <c r="D13" s="2" t="s">
+      <c r="H14" s="5" t="s">
         <v>76</v>
-      </c>
-      <c r="E13" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="F13" s="5"/>
-      <c r="G13" s="10" t="s">
-        <v>77</v>
-      </c>
-      <c r="H13" s="5" t="s">
-        <v>78</v>
-      </c>
-      <c r="I13" s="5"/>
-      <c r="J13" s="5"/>
-      <c r="K13" s="5"/>
-      <c r="L13" s="5"/>
-      <c r="M13" s="5"/>
-      <c r="N13" s="5"/>
-      <c r="O13" s="5"/>
-      <c r="P13" s="5"/>
-      <c r="Q13" s="5"/>
-      <c r="R13" s="5"/>
-      <c r="S13" s="5"/>
-      <c r="T13" s="5"/>
-      <c r="U13" s="5"/>
-      <c r="V13" s="5"/>
-      <c r="W13" s="5"/>
-      <c r="X13" s="5"/>
-      <c r="Y13" s="5"/>
-      <c r="Z13" s="5"/>
-    </row>
-    <row r="14" spans="1:26" s="7" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="5" t="s">
-        <v>83</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="D14" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="E14" s="5" t="s">
-        <v>89</v>
-      </c>
-      <c r="F14" s="5"/>
-      <c r="G14" s="10"/>
-      <c r="H14" s="5" t="s">
-        <v>90</v>
       </c>
       <c r="I14" s="5"/>
       <c r="J14" s="5"/>
@@ -2447,28 +2660,26 @@
       <c r="Y14" s="5"/>
       <c r="Z14" s="5"/>
     </row>
-    <row r="15" spans="1:26" s="6" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="5" t="s">
-        <v>92</v>
+    <row r="15" spans="1:26" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="2" t="s">
+        <v>89</v>
       </c>
       <c r="B15" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="C15" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="C15" s="2" t="s">
-        <v>88</v>
-      </c>
       <c r="D15" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E15" s="5" t="s">
-        <v>51</v>
+        <v>86</v>
       </c>
       <c r="F15" s="5"/>
-      <c r="G15" s="10" t="s">
-        <v>85</v>
-      </c>
+      <c r="G15" s="10"/>
       <c r="H15" s="5" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="I15" s="5"/>
       <c r="J15" s="5"/>
@@ -2490,14 +2701,28 @@
       <c r="Z15" s="5"/>
     </row>
     <row r="16" spans="1:26" s="6" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="5"/>
-      <c r="B16" s="5"/>
-      <c r="C16" s="5"/>
-      <c r="D16" s="5"/>
-      <c r="E16" s="5"/>
+      <c r="A16" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="E16" s="5" t="s">
+        <v>50</v>
+      </c>
       <c r="F16" s="5"/>
-      <c r="G16" s="10"/>
-      <c r="H16" s="5"/>
+      <c r="G16" s="10" t="s">
+        <v>83</v>
+      </c>
+      <c r="H16" s="5" t="s">
+        <v>88</v>
+      </c>
       <c r="I16" s="5"/>
       <c r="J16" s="5"/>
       <c r="K16" s="5"/>
@@ -2518,42 +2743,65 @@
       <c r="Z16" s="5"/>
     </row>
     <row r="17" spans="1:26" s="6" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="5"/>
-      <c r="B17" s="5"/>
-      <c r="C17" s="5"/>
-      <c r="D17" s="5"/>
-      <c r="E17" s="5"/>
-      <c r="F17" s="5"/>
-      <c r="G17" s="10"/>
-      <c r="H17" s="5"/>
-      <c r="I17" s="5"/>
-      <c r="J17" s="5"/>
-      <c r="K17" s="5"/>
-      <c r="L17" s="5"/>
-      <c r="M17" s="5"/>
-      <c r="N17" s="5"/>
-      <c r="O17" s="5"/>
-      <c r="P17" s="5"/>
-      <c r="Q17" s="5"/>
-      <c r="R17" s="5"/>
-      <c r="S17" s="5"/>
-      <c r="T17" s="5"/>
-      <c r="U17" s="5"/>
-      <c r="V17" s="5"/>
-      <c r="W17" s="5"/>
-      <c r="X17" s="5"/>
-      <c r="Y17" s="5"/>
-      <c r="Z17" s="5"/>
+      <c r="A17" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="D17" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="E17" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="F17" s="1"/>
+      <c r="H17" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="I17" s="1"/>
+      <c r="J17" s="1"/>
+      <c r="K17" s="1"/>
+      <c r="L17" s="1"/>
+      <c r="M17" s="1"/>
+      <c r="N17" s="1"/>
+      <c r="O17" s="1"/>
+      <c r="P17" s="1"/>
+      <c r="Q17" s="1"/>
+      <c r="R17" s="1"/>
+      <c r="S17" s="1"/>
+      <c r="T17" s="1"/>
+      <c r="U17" s="1"/>
+      <c r="V17" s="1"/>
+      <c r="W17" s="1"/>
+      <c r="X17" s="1"/>
+      <c r="Y17" s="1"/>
+      <c r="Z17" s="1"/>
     </row>
     <row r="18" spans="1:26" s="6" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="8"/>
-      <c r="B18" s="8"/>
-      <c r="C18" s="8"/>
-      <c r="D18" s="8"/>
-      <c r="E18" s="8"/>
-      <c r="F18" s="8"/>
+      <c r="A18" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="D18" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="E18" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="F18" s="5"/>
       <c r="G18" s="10"/>
-      <c r="H18" s="5"/>
+      <c r="H18" s="5" t="s">
+        <v>99</v>
+      </c>
       <c r="I18" s="5"/>
       <c r="J18" s="5"/>
       <c r="K18" s="5"/>
@@ -2573,33 +2821,33 @@
       <c r="Y18" s="5"/>
       <c r="Z18" s="5"/>
     </row>
-    <row r="19" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A19" s="4"/>
-      <c r="B19" s="4"/>
-      <c r="C19" s="4"/>
-      <c r="D19" s="4"/>
-      <c r="E19" s="4"/>
-      <c r="F19" s="4"/>
-      <c r="G19" s="9"/>
-      <c r="H19" s="1"/>
-      <c r="I19" s="1"/>
-      <c r="J19" s="1"/>
-      <c r="K19" s="1"/>
-      <c r="L19" s="1"/>
-      <c r="M19" s="1"/>
-      <c r="N19" s="1"/>
-      <c r="O19" s="1"/>
-      <c r="P19" s="1"/>
-      <c r="Q19" s="1"/>
-      <c r="R19" s="1"/>
-      <c r="S19" s="1"/>
-      <c r="T19" s="1"/>
-      <c r="U19" s="1"/>
-      <c r="V19" s="1"/>
-      <c r="W19" s="1"/>
-      <c r="X19" s="1"/>
-      <c r="Y19" s="1"/>
-      <c r="Z19" s="1"/>
+    <row r="19" spans="1:26" s="6" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="8"/>
+      <c r="B19" s="8"/>
+      <c r="C19" s="8"/>
+      <c r="D19" s="8"/>
+      <c r="E19" s="8"/>
+      <c r="F19" s="8"/>
+      <c r="G19" s="10"/>
+      <c r="H19" s="5"/>
+      <c r="I19" s="5"/>
+      <c r="J19" s="5"/>
+      <c r="K19" s="5"/>
+      <c r="L19" s="5"/>
+      <c r="M19" s="5"/>
+      <c r="N19" s="5"/>
+      <c r="O19" s="5"/>
+      <c r="P19" s="5"/>
+      <c r="Q19" s="5"/>
+      <c r="R19" s="5"/>
+      <c r="S19" s="5"/>
+      <c r="T19" s="5"/>
+      <c r="U19" s="5"/>
+      <c r="V19" s="5"/>
+      <c r="W19" s="5"/>
+      <c r="X19" s="5"/>
+      <c r="Y19" s="5"/>
+      <c r="Z19" s="5"/>
     </row>
     <row r="20" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A20" s="4"/>
@@ -2635,7 +2883,7 @@
       <c r="C21" s="4"/>
       <c r="D21" s="4"/>
       <c r="E21" s="4"/>
-      <c r="F21" s="1"/>
+      <c r="F21" s="4"/>
       <c r="G21" s="9"/>
       <c r="H21" s="1"/>
       <c r="I21" s="1"/>
@@ -2658,11 +2906,11 @@
       <c r="Z21" s="1"/>
     </row>
     <row r="22" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A22" s="1"/>
-      <c r="B22" s="1"/>
+      <c r="A22" s="4"/>
+      <c r="B22" s="4"/>
       <c r="C22" s="4"/>
-      <c r="D22" s="1"/>
-      <c r="E22" s="1"/>
+      <c r="D22" s="4"/>
+      <c r="E22" s="4"/>
       <c r="F22" s="1"/>
       <c r="G22" s="9"/>
       <c r="H22" s="1"/>
@@ -2688,7 +2936,7 @@
     <row r="23" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A23" s="1"/>
       <c r="B23" s="1"/>
-      <c r="C23" s="1"/>
+      <c r="C23" s="4"/>
       <c r="D23" s="1"/>
       <c r="E23" s="1"/>
       <c r="F23" s="1"/>
@@ -2773,8 +3021,8 @@
       <c r="A26" s="1"/>
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
-      <c r="D26" s="2"/>
-      <c r="E26" s="2"/>
+      <c r="D26" s="1"/>
+      <c r="E26" s="1"/>
       <c r="F26" s="1"/>
       <c r="G26" s="9"/>
       <c r="H26" s="1"/>
@@ -2801,8 +3049,8 @@
       <c r="A27" s="1"/>
       <c r="B27" s="1"/>
       <c r="C27" s="1"/>
-      <c r="D27" s="1"/>
-      <c r="E27" s="1"/>
+      <c r="D27" s="2"/>
+      <c r="E27" s="2"/>
       <c r="F27" s="1"/>
       <c r="G27" s="9"/>
       <c r="H27" s="1"/>
@@ -30097,6 +30345,34 @@
       <c r="Y1001" s="1"/>
       <c r="Z1001" s="1"/>
     </row>
+    <row r="1002" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A1002" s="1"/>
+      <c r="B1002" s="1"/>
+      <c r="C1002" s="1"/>
+      <c r="D1002" s="1"/>
+      <c r="E1002" s="1"/>
+      <c r="F1002" s="1"/>
+      <c r="G1002" s="9"/>
+      <c r="H1002" s="1"/>
+      <c r="I1002" s="1"/>
+      <c r="J1002" s="1"/>
+      <c r="K1002" s="1"/>
+      <c r="L1002" s="1"/>
+      <c r="M1002" s="1"/>
+      <c r="N1002" s="1"/>
+      <c r="O1002" s="1"/>
+      <c r="P1002" s="1"/>
+      <c r="Q1002" s="1"/>
+      <c r="R1002" s="1"/>
+      <c r="S1002" s="1"/>
+      <c r="T1002" s="1"/>
+      <c r="U1002" s="1"/>
+      <c r="V1002" s="1"/>
+      <c r="W1002" s="1"/>
+      <c r="X1002" s="1"/>
+      <c r="Y1002" s="1"/>
+      <c r="Z1002" s="1"/>
+    </row>
   </sheetData>
   <phoneticPr fontId="23" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
fix a bug in special_TR.py
</commit_message>
<xml_diff>
--- a/SSR/SSR-test.xlsx
+++ b/SSR/SSR-test.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bo/Documents/projects/DomainModelExtractor/SSR/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1A73C62-25E9-D746-BF8E-BA369F9B5F4F}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1DE2C6A-32E1-7048-B2C5-0B24F84F6AAA}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="23100" windowHeight="17540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2160" yWindow="460" windowWidth="23100" windowHeight="17540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="update_SSR" sheetId="1" r:id="rId1"/>
@@ -306,47 +306,6 @@
         <family val="2"/>
       </rPr>
       <t>.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">As a gas </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>keeper</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">, I stop </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>filling</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> when the tank's status is full.</t>
     </r>
   </si>
   <si>
@@ -1160,6 +1119,65 @@
   </si>
   <si>
     <t>SVCVO</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">As a </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>gas</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>keeper</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">, I stop </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>filling</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> when the tank's status is full.</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -2069,10 +2087,10 @@
   <dimension ref="A1:Z1002"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="F3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B22" sqref="B22"/>
+      <selection pane="bottomRight" activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2106,10 +2124,10 @@
         <v>14</v>
       </c>
       <c r="G1" s="9" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="I1" s="1"/>
       <c r="J1" s="1"/>
@@ -2135,7 +2153,7 @@
         <v>4</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>18</v>
@@ -2144,7 +2162,7 @@
         <v>17</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F2" s="1"/>
       <c r="G2" s="9" t="s">
@@ -2177,16 +2195,16 @@
         <v>5</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>25</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F3" s="1"/>
       <c r="G3" s="9"/>
@@ -2217,21 +2235,21 @@
         <v>6</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>25</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F4" s="1"/>
       <c r="G4" s="9"/>
       <c r="H4" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="I4" s="1"/>
       <c r="J4" s="1"/>
@@ -2257,7 +2275,7 @@
         <v>7</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>30</v>
@@ -2266,7 +2284,7 @@
         <v>22</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F5" s="1"/>
       <c r="G5" s="9"/>
@@ -2297,7 +2315,7 @@
         <v>8</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>24</v>
@@ -2306,14 +2324,14 @@
         <v>16</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F6" s="1"/>
       <c r="G6" s="9">
         <v>3</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>37</v>
+        <v>107</v>
       </c>
       <c r="I6" s="1"/>
       <c r="J6" s="1"/>
@@ -2339,21 +2357,21 @@
         <v>9</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>31</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F7" s="1"/>
       <c r="G7" s="9"/>
       <c r="H7" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="I7" s="1"/>
       <c r="J7" s="1"/>
@@ -2379,23 +2397,23 @@
         <v>10</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>29</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F8" s="1"/>
       <c r="G8" s="9" t="s">
         <v>32</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="I8" s="1"/>
       <c r="J8" s="1"/>
@@ -2434,10 +2452,10 @@
       </c>
       <c r="F9" s="1"/>
       <c r="G9" s="9" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="I9" s="1"/>
       <c r="J9" s="1"/>
@@ -2463,7 +2481,7 @@
         <v>12</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>28</v>
@@ -2477,7 +2495,7 @@
       <c r="F10" s="1"/>
       <c r="G10" s="9"/>
       <c r="H10" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="I10" s="1"/>
       <c r="J10" s="1"/>
@@ -2503,21 +2521,21 @@
         <v>13</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F11" s="1"/>
       <c r="G11" s="9"/>
       <c r="H11" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="I11" s="1"/>
       <c r="J11" s="1"/>
@@ -2540,24 +2558,24 @@
     </row>
     <row r="12" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B12" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="D12" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="C12" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="D12" s="3" t="s">
-        <v>65</v>
-      </c>
       <c r="E12" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F12" s="1"/>
       <c r="G12" s="9"/>
       <c r="H12" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="I12" s="1"/>
       <c r="J12" s="1"/>
@@ -2580,24 +2598,24 @@
     </row>
     <row r="13" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B13" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C13" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="C13" s="1" t="s">
-        <v>67</v>
-      </c>
       <c r="D13" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F13" s="1"/>
       <c r="G13" s="9"/>
       <c r="H13" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="I13" s="1"/>
       <c r="J13" s="1"/>
@@ -2620,26 +2638,26 @@
     </row>
     <row r="14" spans="1:26" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B14" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="C14" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="C14" s="2" t="s">
+      <c r="D14" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="D14" s="2" t="s">
-        <v>74</v>
-      </c>
       <c r="E14" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F14" s="5"/>
       <c r="G14" s="10" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="H14" s="5" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="I14" s="5"/>
       <c r="J14" s="5"/>
@@ -2662,24 +2680,24 @@
     </row>
     <row r="15" spans="1:26" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E15" s="5" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F15" s="5"/>
       <c r="G15" s="10"/>
       <c r="H15" s="5" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="I15" s="5"/>
       <c r="J15" s="5"/>
@@ -2702,26 +2720,26 @@
     </row>
     <row r="16" spans="1:26" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E16" s="5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F16" s="5"/>
       <c r="G16" s="10" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="H16" s="5" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="I16" s="5"/>
       <c r="J16" s="5"/>
@@ -2744,23 +2762,23 @@
     </row>
     <row r="17" spans="1:26" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="C17" s="4" t="s">
         <v>93</v>
       </c>
-      <c r="B17" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="C17" s="4" t="s">
-        <v>94</v>
-      </c>
       <c r="D17" s="4" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E17" s="4" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F17" s="1"/>
       <c r="H17" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="I17" s="1"/>
       <c r="J17" s="1"/>
@@ -2783,24 +2801,24 @@
     </row>
     <row r="18" spans="1:26" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B18" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="D18" s="4" t="s">
         <v>96</v>
       </c>
-      <c r="C18" s="4" t="s">
-        <v>95</v>
-      </c>
-      <c r="D18" s="4" t="s">
+      <c r="E18" s="4" t="s">
         <v>97</v>
-      </c>
-      <c r="E18" s="4" t="s">
-        <v>98</v>
       </c>
       <c r="F18" s="5"/>
       <c r="G18" s="10"/>
       <c r="H18" s="5" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="I18" s="5"/>
       <c r="J18" s="5"/>

</xml_diff>

<commit_message>
Revert "Merge branch '2021s' of https://github.com/xixixhalu/DomainModelExtractor into 2021s"
This reverts commit 6de3b1478366f4bd021362be56e77f4385c61b81, reversing
changes made to 7054a6cf6e452157a4b9606e6f981a1d6be8f9ba.
</commit_message>
<xml_diff>
--- a/SSR/SSR-test.xlsx
+++ b/SSR/SSR-test.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bo/Documents/projects/DomainModelExtractor/SSR/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1DE2C6A-32E1-7048-B2C5-0B24F84F6AAA}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D20D8ABC-724C-9F47-80B0-38481F559F73}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2160" yWindow="460" windowWidth="23100" windowHeight="17540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="23100" windowHeight="17540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="update_SSR" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="93">
   <si>
     <t>Rule</t>
   </si>
@@ -310,6 +310,47 @@
   </si>
   <si>
     <r>
+      <t xml:space="preserve">As a gas </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>keeper</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">, I stop </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>filling</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> when the tank's status is full.</t>
+    </r>
+  </si>
+  <si>
+    <r>
       <t xml:space="preserve">As a </t>
     </r>
     <r>
@@ -473,6 +514,9 @@
     </r>
   </si>
   <si>
+    <t>nsubj(A,B), obl*(A,C)</t>
+  </si>
+  <si>
     <t>Sentence Example</t>
   </si>
   <si>
@@ -501,6 +545,9 @@
   </si>
   <si>
     <t>SVObj</t>
+  </si>
+  <si>
+    <t>SVObl</t>
   </si>
   <si>
     <t>SVCcO</t>
@@ -787,6 +834,9 @@
     <t>12</t>
   </si>
   <si>
+    <t>1, 2, 3, 4, 5, 6, 10, 11, 12, 13</t>
+  </si>
+  <si>
     <t>Subject-Verb-By-Verb-Object</t>
   </si>
   <si>
@@ -897,287 +947,6 @@
   </si>
   <si>
     <t>SSR14</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">As a </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>seller</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">, I can replace, </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>buy</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> and </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>sell</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> phones.</t>
-    </r>
-  </si>
-  <si>
-    <t>SSR15</t>
-  </si>
-  <si>
-    <t>nsubj(A,B), conj*(A,C), obj(A,D)</t>
-  </si>
-  <si>
-    <t>SSR16</t>
-  </si>
-  <si>
-    <t>Subject-Verb-CC-Verb-Object</t>
-  </si>
-  <si>
-    <t>Noun-ClausalModifier</t>
-  </si>
-  <si>
-    <t>AO</t>
-  </si>
-  <si>
-    <t>acl(A,B), obj(B,C)</t>
-  </si>
-  <si>
-    <t>A==NN*, B==VBG, C==NN*</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">As a GM, I can make </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>decision</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>affecting</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>results</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>.</t>
-    </r>
-  </si>
-  <si>
-    <t>nsubj(A,B), obl:on(A,C)</t>
-  </si>
-  <si>
-    <t>SVOblIn</t>
-  </si>
-  <si>
-    <t>SVOblOn</t>
-  </si>
-  <si>
-    <t>nsubj(A,B), obl:in(A,C)</t>
-  </si>
-  <si>
-    <t>SSR17</t>
-  </si>
-  <si>
-    <t>1, 2, 3, 4, 5, 6, 7, 11, 12, 13, 14, 15, 16</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">As a </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>student</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">, I </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>work</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> in an </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>university</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>.</t>
-    </r>
-  </si>
-  <si>
-    <t>SVCVO</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">As a </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>gas</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>keeper</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">, I stop </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>filling</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> when the tank's status is full.</t>
-    </r>
   </si>
 </sst>
 </file>
@@ -2084,13 +1853,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z1002"/>
+  <dimension ref="A1:Z1001"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D22" sqref="D22"/>
+      <selection pane="bottomRight" activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2124,10 +1893,10 @@
         <v>14</v>
       </c>
       <c r="G1" s="9" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="I1" s="1"/>
       <c r="J1" s="1"/>
@@ -2153,7 +1922,7 @@
         <v>4</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>18</v>
@@ -2162,7 +1931,7 @@
         <v>17</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="F2" s="1"/>
       <c r="G2" s="9" t="s">
@@ -2195,16 +1964,16 @@
         <v>5</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>101</v>
+        <v>53</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>25</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>99</v>
+        <v>42</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="F3" s="1"/>
       <c r="G3" s="9"/>
@@ -2230,26 +1999,26 @@
       <c r="Y3" s="1"/>
       <c r="Z3" s="1"/>
     </row>
-    <row r="4" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A4" s="2" t="s">
+    <row r="4" spans="1:26" s="6" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>100</v>
+        <v>54</v>
       </c>
-      <c r="C4" s="2" t="s">
-        <v>25</v>
+      <c r="C4" s="1" t="s">
+        <v>30</v>
       </c>
-      <c r="D4" s="2" t="s">
-        <v>102</v>
+      <c r="D4" s="3" t="s">
+        <v>22</v>
       </c>
-      <c r="E4" s="2" t="s">
-        <v>47</v>
+      <c r="E4" s="1" t="s">
+        <v>50</v>
       </c>
       <c r="F4" s="1"/>
       <c r="G4" s="9"/>
       <c r="H4" s="1" t="s">
-        <v>105</v>
+        <v>36</v>
       </c>
       <c r="I4" s="1"/>
       <c r="J4" s="1"/>
@@ -2270,26 +2039,28 @@
       <c r="Y4" s="1"/>
       <c r="Z4" s="1"/>
     </row>
-    <row r="5" spans="1:26" s="6" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="2" t="s">
+    <row r="5" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E5" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="C5" s="1" t="s">
-        <v>30</v>
+      <c r="F5" s="1"/>
+      <c r="G5" s="9">
+        <v>3</v>
       </c>
-      <c r="D5" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="F5" s="1"/>
-      <c r="G5" s="9"/>
       <c r="H5" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="I5" s="1"/>
       <c r="J5" s="1"/>
@@ -2311,27 +2082,25 @@
       <c r="Z5" s="1"/>
     </row>
     <row r="6" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A6" s="2" t="s">
+      <c r="A6" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>24</v>
+        <v>31</v>
       </c>
-      <c r="D6" s="2" t="s">
-        <v>16</v>
+      <c r="D6" s="3" t="s">
+        <v>45</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="F6" s="1"/>
-      <c r="G6" s="9">
-        <v>3</v>
-      </c>
+      <c r="G6" s="9"/>
       <c r="H6" s="1" t="s">
-        <v>107</v>
+        <v>38</v>
       </c>
       <c r="I6" s="1"/>
       <c r="J6" s="1"/>
@@ -2353,25 +2122,27 @@
       <c r="Z6" s="1"/>
     </row>
     <row r="7" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A7" s="2" t="s">
+      <c r="A7" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="F7" s="1"/>
-      <c r="G7" s="9"/>
+      <c r="G7" s="9" t="s">
+        <v>32</v>
+      </c>
       <c r="H7" s="1" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="I7" s="1"/>
       <c r="J7" s="1"/>
@@ -2393,27 +2164,27 @@
       <c r="Z7" s="1"/>
     </row>
     <row r="8" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A8" s="2" t="s">
+      <c r="A8" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>54</v>
+        <v>19</v>
       </c>
-      <c r="C8" s="2" t="s">
-        <v>29</v>
+      <c r="C8" s="1" t="s">
+        <v>20</v>
       </c>
-      <c r="D8" s="3" t="s">
-        <v>44</v>
+      <c r="D8" s="1" t="s">
+        <v>21</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>46</v>
+        <v>23</v>
       </c>
       <c r="F8" s="1"/>
       <c r="G8" s="9" t="s">
-        <v>32</v>
+        <v>86</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="I8" s="1"/>
       <c r="J8" s="1"/>
@@ -2435,27 +2206,25 @@
       <c r="Z8" s="1"/>
     </row>
     <row r="9" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A9" s="2" t="s">
+      <c r="A9" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>19</v>
+        <v>58</v>
       </c>
-      <c r="C9" s="1" t="s">
-        <v>20</v>
+      <c r="C9" s="2" t="s">
+        <v>28</v>
       </c>
-      <c r="D9" s="1" t="s">
-        <v>21</v>
+      <c r="D9" s="3" t="s">
+        <v>26</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="F9" s="1"/>
-      <c r="G9" s="9" t="s">
-        <v>104</v>
-      </c>
+      <c r="G9" s="9"/>
       <c r="H9" s="1" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="I9" s="1"/>
       <c r="J9" s="1"/>
@@ -2477,25 +2246,25 @@
       <c r="Z9" s="1"/>
     </row>
     <row r="10" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A10" s="2" t="s">
+      <c r="A10" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>55</v>
+        <v>62</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>28</v>
+        <v>61</v>
       </c>
-      <c r="D10" s="3" t="s">
-        <v>26</v>
+      <c r="D10" s="2" t="s">
+        <v>59</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>27</v>
+        <v>60</v>
       </c>
       <c r="F10" s="1"/>
       <c r="G10" s="9"/>
       <c r="H10" s="1" t="s">
-        <v>40</v>
+        <v>63</v>
       </c>
       <c r="I10" s="1"/>
       <c r="J10" s="1"/>
@@ -2517,25 +2286,25 @@
       <c r="Z10" s="1"/>
     </row>
     <row r="11" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A11" s="2" t="s">
+      <c r="A11" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B11" s="1" t="s">
-        <v>59</v>
+      <c r="B11" s="2" t="s">
+        <v>66</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>58</v>
+        <v>65</v>
       </c>
-      <c r="D11" s="2" t="s">
-        <v>56</v>
+      <c r="D11" s="3" t="s">
+        <v>67</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="F11" s="1"/>
       <c r="G11" s="9"/>
       <c r="H11" s="1" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="I11" s="1"/>
       <c r="J11" s="1"/>
@@ -2557,25 +2326,25 @@
       <c r="Z11" s="1"/>
     </row>
     <row r="12" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A12" s="2" t="s">
-        <v>70</v>
+      <c r="A12" s="5" t="s">
+        <v>73</v>
       </c>
-      <c r="B12" s="2" t="s">
-        <v>63</v>
+      <c r="B12" s="1" t="s">
+        <v>68</v>
       </c>
-      <c r="C12" s="2" t="s">
-        <v>62</v>
+      <c r="C12" s="1" t="s">
+        <v>69</v>
       </c>
-      <c r="D12" s="3" t="s">
-        <v>64</v>
+      <c r="D12" s="1" t="s">
+        <v>71</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>49</v>
+        <v>72</v>
       </c>
       <c r="F12" s="1"/>
       <c r="G12" s="9"/>
       <c r="H12" s="1" t="s">
-        <v>61</v>
+        <v>70</v>
       </c>
       <c r="I12" s="1"/>
       <c r="J12" s="1"/>
@@ -2596,68 +2365,68 @@
       <c r="Y12" s="1"/>
       <c r="Z12" s="1"/>
     </row>
-    <row r="13" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A13" s="2" t="s">
+    <row r="13" spans="1:26" s="6" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="D13" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="B13" s="1" t="s">
-        <v>65</v>
+      <c r="E13" s="2" t="s">
+        <v>49</v>
       </c>
-      <c r="C13" s="1" t="s">
-        <v>66</v>
+      <c r="F13" s="5"/>
+      <c r="G13" s="10" t="s">
+        <v>77</v>
       </c>
-      <c r="D13" s="1" t="s">
-        <v>68</v>
+      <c r="H13" s="5" t="s">
+        <v>78</v>
       </c>
-      <c r="E13" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="F13" s="1"/>
-      <c r="G13" s="9"/>
-      <c r="H13" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="I13" s="1"/>
-      <c r="J13" s="1"/>
-      <c r="K13" s="1"/>
-      <c r="L13" s="1"/>
-      <c r="M13" s="1"/>
-      <c r="N13" s="1"/>
-      <c r="O13" s="1"/>
-      <c r="P13" s="1"/>
-      <c r="Q13" s="1"/>
-      <c r="R13" s="1"/>
-      <c r="S13" s="1"/>
-      <c r="T13" s="1"/>
-      <c r="U13" s="1"/>
-      <c r="V13" s="1"/>
-      <c r="W13" s="1"/>
-      <c r="X13" s="1"/>
-      <c r="Y13" s="1"/>
-      <c r="Z13" s="1"/>
-    </row>
-    <row r="14" spans="1:26" s="6" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="2" t="s">
-        <v>80</v>
+      <c r="I13" s="5"/>
+      <c r="J13" s="5"/>
+      <c r="K13" s="5"/>
+      <c r="L13" s="5"/>
+      <c r="M13" s="5"/>
+      <c r="N13" s="5"/>
+      <c r="O13" s="5"/>
+      <c r="P13" s="5"/>
+      <c r="Q13" s="5"/>
+      <c r="R13" s="5"/>
+      <c r="S13" s="5"/>
+      <c r="T13" s="5"/>
+      <c r="U13" s="5"/>
+      <c r="V13" s="5"/>
+      <c r="W13" s="5"/>
+      <c r="X13" s="5"/>
+      <c r="Y13" s="5"/>
+      <c r="Z13" s="5"/>
+    </row>
+    <row r="14" spans="1:26" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="5" t="s">
+        <v>83</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>71</v>
+        <v>82</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>72</v>
+        <v>87</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>73</v>
+        <v>81</v>
       </c>
-      <c r="E14" s="2" t="s">
-        <v>47</v>
+      <c r="E14" s="5" t="s">
+        <v>89</v>
       </c>
       <c r="F14" s="5"/>
-      <c r="G14" s="10" t="s">
-        <v>74</v>
-      </c>
+      <c r="G14" s="10"/>
       <c r="H14" s="5" t="s">
-        <v>75</v>
+        <v>90</v>
       </c>
       <c r="I14" s="5"/>
       <c r="J14" s="5"/>
@@ -2678,26 +2447,28 @@
       <c r="Y14" s="5"/>
       <c r="Z14" s="5"/>
     </row>
-    <row r="15" spans="1:26" s="7" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="2" t="s">
+    <row r="15" spans="1:26" s="6" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="C15" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="B15" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>83</v>
-      </c>
       <c r="D15" s="2" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="E15" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="F15" s="5"/>
+      <c r="G15" s="10" t="s">
         <v>85</v>
       </c>
-      <c r="F15" s="5"/>
-      <c r="G15" s="10"/>
       <c r="H15" s="5" t="s">
-        <v>86</v>
+        <v>91</v>
       </c>
       <c r="I15" s="5"/>
       <c r="J15" s="5"/>
@@ -2719,28 +2490,14 @@
       <c r="Z15" s="5"/>
     </row>
     <row r="16" spans="1:26" s="6" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="D16" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="E16" s="5" t="s">
-        <v>49</v>
-      </c>
+      <c r="A16" s="5"/>
+      <c r="B16" s="5"/>
+      <c r="C16" s="5"/>
+      <c r="D16" s="5"/>
+      <c r="E16" s="5"/>
       <c r="F16" s="5"/>
-      <c r="G16" s="10" t="s">
-        <v>82</v>
-      </c>
-      <c r="H16" s="5" t="s">
-        <v>87</v>
-      </c>
+      <c r="G16" s="10"/>
+      <c r="H16" s="5"/>
       <c r="I16" s="5"/>
       <c r="J16" s="5"/>
       <c r="K16" s="5"/>
@@ -2761,65 +2518,42 @@
       <c r="Z16" s="5"/>
     </row>
     <row r="17" spans="1:26" s="6" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="C17" s="4" t="s">
-        <v>93</v>
-      </c>
-      <c r="D17" s="4" t="s">
-        <v>91</v>
-      </c>
-      <c r="E17" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="F17" s="1"/>
-      <c r="H17" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="I17" s="1"/>
-      <c r="J17" s="1"/>
-      <c r="K17" s="1"/>
-      <c r="L17" s="1"/>
-      <c r="M17" s="1"/>
-      <c r="N17" s="1"/>
-      <c r="O17" s="1"/>
-      <c r="P17" s="1"/>
-      <c r="Q17" s="1"/>
-      <c r="R17" s="1"/>
-      <c r="S17" s="1"/>
-      <c r="T17" s="1"/>
-      <c r="U17" s="1"/>
-      <c r="V17" s="1"/>
-      <c r="W17" s="1"/>
-      <c r="X17" s="1"/>
-      <c r="Y17" s="1"/>
-      <c r="Z17" s="1"/>
+      <c r="A17" s="5"/>
+      <c r="B17" s="5"/>
+      <c r="C17" s="5"/>
+      <c r="D17" s="5"/>
+      <c r="E17" s="5"/>
+      <c r="F17" s="5"/>
+      <c r="G17" s="10"/>
+      <c r="H17" s="5"/>
+      <c r="I17" s="5"/>
+      <c r="J17" s="5"/>
+      <c r="K17" s="5"/>
+      <c r="L17" s="5"/>
+      <c r="M17" s="5"/>
+      <c r="N17" s="5"/>
+      <c r="O17" s="5"/>
+      <c r="P17" s="5"/>
+      <c r="Q17" s="5"/>
+      <c r="R17" s="5"/>
+      <c r="S17" s="5"/>
+      <c r="T17" s="5"/>
+      <c r="U17" s="5"/>
+      <c r="V17" s="5"/>
+      <c r="W17" s="5"/>
+      <c r="X17" s="5"/>
+      <c r="Y17" s="5"/>
+      <c r="Z17" s="5"/>
     </row>
     <row r="18" spans="1:26" s="6" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="C18" s="4" t="s">
-        <v>94</v>
-      </c>
-      <c r="D18" s="4" t="s">
-        <v>96</v>
-      </c>
-      <c r="E18" s="4" t="s">
-        <v>97</v>
-      </c>
-      <c r="F18" s="5"/>
+      <c r="A18" s="8"/>
+      <c r="B18" s="8"/>
+      <c r="C18" s="8"/>
+      <c r="D18" s="8"/>
+      <c r="E18" s="8"/>
+      <c r="F18" s="8"/>
       <c r="G18" s="10"/>
-      <c r="H18" s="5" t="s">
-        <v>98</v>
-      </c>
+      <c r="H18" s="5"/>
       <c r="I18" s="5"/>
       <c r="J18" s="5"/>
       <c r="K18" s="5"/>
@@ -2839,33 +2573,33 @@
       <c r="Y18" s="5"/>
       <c r="Z18" s="5"/>
     </row>
-    <row r="19" spans="1:26" s="6" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="8"/>
-      <c r="B19" s="8"/>
-      <c r="C19" s="8"/>
-      <c r="D19" s="8"/>
-      <c r="E19" s="8"/>
-      <c r="F19" s="8"/>
-      <c r="G19" s="10"/>
-      <c r="H19" s="5"/>
-      <c r="I19" s="5"/>
-      <c r="J19" s="5"/>
-      <c r="K19" s="5"/>
-      <c r="L19" s="5"/>
-      <c r="M19" s="5"/>
-      <c r="N19" s="5"/>
-      <c r="O19" s="5"/>
-      <c r="P19" s="5"/>
-      <c r="Q19" s="5"/>
-      <c r="R19" s="5"/>
-      <c r="S19" s="5"/>
-      <c r="T19" s="5"/>
-      <c r="U19" s="5"/>
-      <c r="V19" s="5"/>
-      <c r="W19" s="5"/>
-      <c r="X19" s="5"/>
-      <c r="Y19" s="5"/>
-      <c r="Z19" s="5"/>
+    <row r="19" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A19" s="4"/>
+      <c r="B19" s="4"/>
+      <c r="C19" s="4"/>
+      <c r="D19" s="4"/>
+      <c r="E19" s="4"/>
+      <c r="F19" s="4"/>
+      <c r="G19" s="9"/>
+      <c r="H19" s="1"/>
+      <c r="I19" s="1"/>
+      <c r="J19" s="1"/>
+      <c r="K19" s="1"/>
+      <c r="L19" s="1"/>
+      <c r="M19" s="1"/>
+      <c r="N19" s="1"/>
+      <c r="O19" s="1"/>
+      <c r="P19" s="1"/>
+      <c r="Q19" s="1"/>
+      <c r="R19" s="1"/>
+      <c r="S19" s="1"/>
+      <c r="T19" s="1"/>
+      <c r="U19" s="1"/>
+      <c r="V19" s="1"/>
+      <c r="W19" s="1"/>
+      <c r="X19" s="1"/>
+      <c r="Y19" s="1"/>
+      <c r="Z19" s="1"/>
     </row>
     <row r="20" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A20" s="4"/>
@@ -2901,7 +2635,7 @@
       <c r="C21" s="4"/>
       <c r="D21" s="4"/>
       <c r="E21" s="4"/>
-      <c r="F21" s="4"/>
+      <c r="F21" s="1"/>
       <c r="G21" s="9"/>
       <c r="H21" s="1"/>
       <c r="I21" s="1"/>
@@ -2924,11 +2658,11 @@
       <c r="Z21" s="1"/>
     </row>
     <row r="22" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A22" s="4"/>
-      <c r="B22" s="4"/>
+      <c r="A22" s="1"/>
+      <c r="B22" s="1"/>
       <c r="C22" s="4"/>
-      <c r="D22" s="4"/>
-      <c r="E22" s="4"/>
+      <c r="D22" s="1"/>
+      <c r="E22" s="1"/>
       <c r="F22" s="1"/>
       <c r="G22" s="9"/>
       <c r="H22" s="1"/>
@@ -2954,7 +2688,7 @@
     <row r="23" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A23" s="1"/>
       <c r="B23" s="1"/>
-      <c r="C23" s="4"/>
+      <c r="C23" s="1"/>
       <c r="D23" s="1"/>
       <c r="E23" s="1"/>
       <c r="F23" s="1"/>
@@ -3039,8 +2773,8 @@
       <c r="A26" s="1"/>
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
-      <c r="D26" s="1"/>
-      <c r="E26" s="1"/>
+      <c r="D26" s="2"/>
+      <c r="E26" s="2"/>
       <c r="F26" s="1"/>
       <c r="G26" s="9"/>
       <c r="H26" s="1"/>
@@ -3067,8 +2801,8 @@
       <c r="A27" s="1"/>
       <c r="B27" s="1"/>
       <c r="C27" s="1"/>
-      <c r="D27" s="2"/>
-      <c r="E27" s="2"/>
+      <c r="D27" s="1"/>
+      <c r="E27" s="1"/>
       <c r="F27" s="1"/>
       <c r="G27" s="9"/>
       <c r="H27" s="1"/>
@@ -30363,34 +30097,6 @@
       <c r="Y1001" s="1"/>
       <c r="Z1001" s="1"/>
     </row>
-    <row r="1002" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A1002" s="1"/>
-      <c r="B1002" s="1"/>
-      <c r="C1002" s="1"/>
-      <c r="D1002" s="1"/>
-      <c r="E1002" s="1"/>
-      <c r="F1002" s="1"/>
-      <c r="G1002" s="9"/>
-      <c r="H1002" s="1"/>
-      <c r="I1002" s="1"/>
-      <c r="J1002" s="1"/>
-      <c r="K1002" s="1"/>
-      <c r="L1002" s="1"/>
-      <c r="M1002" s="1"/>
-      <c r="N1002" s="1"/>
-      <c r="O1002" s="1"/>
-      <c r="P1002" s="1"/>
-      <c r="Q1002" s="1"/>
-      <c r="R1002" s="1"/>
-      <c r="S1002" s="1"/>
-      <c r="T1002" s="1"/>
-      <c r="U1002" s="1"/>
-      <c r="V1002" s="1"/>
-      <c r="W1002" s="1"/>
-      <c r="X1002" s="1"/>
-      <c r="Y1002" s="1"/>
-      <c r="Z1002" s="1"/>
-    </row>
   </sheetData>
   <phoneticPr fontId="23" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Revert "Revert "Merge branch '2021s' of https://github.com/xixixhalu/DomainModelExtractor into 2021s""
This reverts commit 0e0b23ff88205dd211dc8e9c9c61ccd74ee7eaba.
</commit_message>
<xml_diff>
--- a/SSR/SSR-test.xlsx
+++ b/SSR/SSR-test.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bo/Documents/projects/DomainModelExtractor/SSR/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D20D8ABC-724C-9F47-80B0-38481F559F73}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1DE2C6A-32E1-7048-B2C5-0B24F84F6AAA}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="23100" windowHeight="17540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2160" yWindow="460" windowWidth="23100" windowHeight="17540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="update_SSR" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="108">
   <si>
     <t>Rule</t>
   </si>
@@ -310,47 +310,6 @@
   </si>
   <si>
     <r>
-      <t xml:space="preserve">As a gas </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>keeper</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">, I stop </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>filling</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> when the tank's status is full.</t>
-    </r>
-  </si>
-  <si>
-    <r>
       <t xml:space="preserve">As a </t>
     </r>
     <r>
@@ -514,9 +473,6 @@
     </r>
   </si>
   <si>
-    <t>nsubj(A,B), obl*(A,C)</t>
-  </si>
-  <si>
     <t>Sentence Example</t>
   </si>
   <si>
@@ -545,9 +501,6 @@
   </si>
   <si>
     <t>SVObj</t>
-  </si>
-  <si>
-    <t>SVObl</t>
   </si>
   <si>
     <t>SVCcO</t>
@@ -834,9 +787,6 @@
     <t>12</t>
   </si>
   <si>
-    <t>1, 2, 3, 4, 5, 6, 10, 11, 12, 13</t>
-  </si>
-  <si>
     <t>Subject-Verb-By-Verb-Object</t>
   </si>
   <si>
@@ -947,6 +897,287 @@
   </si>
   <si>
     <t>SSR14</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">As a </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>seller</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">, I can replace, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>buy</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> and </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>sell</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> phones.</t>
+    </r>
+  </si>
+  <si>
+    <t>SSR15</t>
+  </si>
+  <si>
+    <t>nsubj(A,B), conj*(A,C), obj(A,D)</t>
+  </si>
+  <si>
+    <t>SSR16</t>
+  </si>
+  <si>
+    <t>Subject-Verb-CC-Verb-Object</t>
+  </si>
+  <si>
+    <t>Noun-ClausalModifier</t>
+  </si>
+  <si>
+    <t>AO</t>
+  </si>
+  <si>
+    <t>acl(A,B), obj(B,C)</t>
+  </si>
+  <si>
+    <t>A==NN*, B==VBG, C==NN*</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">As a GM, I can make </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>decision</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>affecting</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>results</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>.</t>
+    </r>
+  </si>
+  <si>
+    <t>nsubj(A,B), obl:on(A,C)</t>
+  </si>
+  <si>
+    <t>SVOblIn</t>
+  </si>
+  <si>
+    <t>SVOblOn</t>
+  </si>
+  <si>
+    <t>nsubj(A,B), obl:in(A,C)</t>
+  </si>
+  <si>
+    <t>SSR17</t>
+  </si>
+  <si>
+    <t>1, 2, 3, 4, 5, 6, 7, 11, 12, 13, 14, 15, 16</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">As a </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>student</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">, I </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>work</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> in an </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>university</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>.</t>
+    </r>
+  </si>
+  <si>
+    <t>SVCVO</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">As a </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>gas</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>keeper</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">, I stop </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>filling</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> when the tank's status is full.</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -1853,13 +2084,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z1001"/>
+  <dimension ref="A1:Z1002"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A15" sqref="A15"/>
+      <selection pane="bottomRight" activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1893,10 +2124,10 @@
         <v>14</v>
       </c>
       <c r="G1" s="9" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="I1" s="1"/>
       <c r="J1" s="1"/>
@@ -1922,7 +2153,7 @@
         <v>4</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>18</v>
@@ -1931,7 +2162,7 @@
         <v>17</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="F2" s="1"/>
       <c r="G2" s="9" t="s">
@@ -1964,16 +2195,16 @@
         <v>5</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>53</v>
+        <v>101</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>25</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>42</v>
+        <v>99</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="F3" s="1"/>
       <c r="G3" s="9"/>
@@ -1999,26 +2230,26 @@
       <c r="Y3" s="1"/>
       <c r="Z3" s="1"/>
     </row>
-    <row r="4" spans="1:26" s="6" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="1" t="s">
+    <row r="4" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A4" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>54</v>
+        <v>100</v>
       </c>
-      <c r="C4" s="1" t="s">
-        <v>30</v>
+      <c r="C4" s="2" t="s">
+        <v>25</v>
       </c>
-      <c r="D4" s="3" t="s">
-        <v>22</v>
+      <c r="D4" s="2" t="s">
+        <v>102</v>
       </c>
-      <c r="E4" s="1" t="s">
-        <v>50</v>
+      <c r="E4" s="2" t="s">
+        <v>47</v>
       </c>
       <c r="F4" s="1"/>
       <c r="G4" s="9"/>
       <c r="H4" s="1" t="s">
-        <v>36</v>
+        <v>105</v>
       </c>
       <c r="I4" s="1"/>
       <c r="J4" s="1"/>
@@ -2039,28 +2270,26 @@
       <c r="Y4" s="1"/>
       <c r="Z4" s="1"/>
     </row>
-    <row r="5" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A5" s="1" t="s">
+    <row r="5" spans="1:26" s="6" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="1" t="s">
-        <v>55</v>
+      <c r="B5" s="2" t="s">
+        <v>51</v>
       </c>
-      <c r="C5" s="2" t="s">
-        <v>24</v>
+      <c r="C5" s="1" t="s">
+        <v>30</v>
       </c>
-      <c r="D5" s="2" t="s">
-        <v>16</v>
+      <c r="D5" s="3" t="s">
+        <v>22</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="F5" s="1"/>
-      <c r="G5" s="9">
-        <v>3</v>
-      </c>
+      <c r="G5" s="9"/>
       <c r="H5" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="I5" s="1"/>
       <c r="J5" s="1"/>
@@ -2082,25 +2311,27 @@
       <c r="Z5" s="1"/>
     </row>
     <row r="6" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A6" s="1" t="s">
+      <c r="A6" s="2" t="s">
         <v>8</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
-      <c r="D6" s="3" t="s">
-        <v>45</v>
+      <c r="D6" s="2" t="s">
+        <v>16</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="F6" s="1"/>
-      <c r="G6" s="9"/>
+      <c r="G6" s="9">
+        <v>3</v>
+      </c>
       <c r="H6" s="1" t="s">
-        <v>38</v>
+        <v>107</v>
       </c>
       <c r="I6" s="1"/>
       <c r="J6" s="1"/>
@@ -2122,27 +2353,25 @@
       <c r="Z6" s="1"/>
     </row>
     <row r="7" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A7" s="1" t="s">
+      <c r="A7" s="2" t="s">
         <v>9</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="F7" s="1"/>
-      <c r="G7" s="9" t="s">
-        <v>32</v>
-      </c>
+      <c r="G7" s="9"/>
       <c r="H7" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="I7" s="1"/>
       <c r="J7" s="1"/>
@@ -2164,27 +2393,27 @@
       <c r="Z7" s="1"/>
     </row>
     <row r="8" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A8" s="1" t="s">
+      <c r="A8" s="2" t="s">
         <v>10</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>19</v>
+        <v>54</v>
       </c>
-      <c r="C8" s="1" t="s">
-        <v>20</v>
+      <c r="C8" s="2" t="s">
+        <v>29</v>
       </c>
-      <c r="D8" s="1" t="s">
-        <v>21</v>
+      <c r="D8" s="3" t="s">
+        <v>44</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>23</v>
+        <v>46</v>
       </c>
       <c r="F8" s="1"/>
       <c r="G8" s="9" t="s">
-        <v>86</v>
+        <v>32</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="I8" s="1"/>
       <c r="J8" s="1"/>
@@ -2206,25 +2435,27 @@
       <c r="Z8" s="1"/>
     </row>
     <row r="9" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A9" s="1" t="s">
+      <c r="A9" s="2" t="s">
         <v>11</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>58</v>
+        <v>19</v>
       </c>
-      <c r="C9" s="2" t="s">
-        <v>28</v>
+      <c r="C9" s="1" t="s">
+        <v>20</v>
       </c>
-      <c r="D9" s="3" t="s">
-        <v>26</v>
+      <c r="D9" s="1" t="s">
+        <v>21</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="F9" s="1"/>
-      <c r="G9" s="9"/>
+      <c r="G9" s="9" t="s">
+        <v>104</v>
+      </c>
       <c r="H9" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="I9" s="1"/>
       <c r="J9" s="1"/>
@@ -2246,25 +2477,25 @@
       <c r="Z9" s="1"/>
     </row>
     <row r="10" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A10" s="1" t="s">
+      <c r="A10" s="2" t="s">
         <v>12</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>62</v>
+        <v>55</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>61</v>
+        <v>28</v>
       </c>
-      <c r="D10" s="2" t="s">
-        <v>59</v>
+      <c r="D10" s="3" t="s">
+        <v>26</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>60</v>
+        <v>27</v>
       </c>
       <c r="F10" s="1"/>
       <c r="G10" s="9"/>
       <c r="H10" s="1" t="s">
-        <v>63</v>
+        <v>40</v>
       </c>
       <c r="I10" s="1"/>
       <c r="J10" s="1"/>
@@ -2286,25 +2517,25 @@
       <c r="Z10" s="1"/>
     </row>
     <row r="11" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A11" s="1" t="s">
+      <c r="A11" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B11" s="2" t="s">
-        <v>66</v>
+      <c r="B11" s="1" t="s">
+        <v>59</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
-      <c r="D11" s="3" t="s">
-        <v>67</v>
+      <c r="D11" s="2" t="s">
+        <v>56</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>51</v>
+        <v>57</v>
       </c>
       <c r="F11" s="1"/>
       <c r="G11" s="9"/>
       <c r="H11" s="1" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="I11" s="1"/>
       <c r="J11" s="1"/>
@@ -2326,25 +2557,25 @@
       <c r="Z11" s="1"/>
     </row>
     <row r="12" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A12" s="5" t="s">
-        <v>73</v>
+      <c r="A12" s="2" t="s">
+        <v>70</v>
       </c>
-      <c r="B12" s="1" t="s">
-        <v>68</v>
+      <c r="B12" s="2" t="s">
+        <v>63</v>
       </c>
-      <c r="C12" s="1" t="s">
-        <v>69</v>
+      <c r="C12" s="2" t="s">
+        <v>62</v>
       </c>
-      <c r="D12" s="1" t="s">
-        <v>71</v>
+      <c r="D12" s="3" t="s">
+        <v>64</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>72</v>
+        <v>49</v>
       </c>
       <c r="F12" s="1"/>
       <c r="G12" s="9"/>
       <c r="H12" s="1" t="s">
-        <v>70</v>
+        <v>61</v>
       </c>
       <c r="I12" s="1"/>
       <c r="J12" s="1"/>
@@ -2365,68 +2596,68 @@
       <c r="Y12" s="1"/>
       <c r="Z12" s="1"/>
     </row>
-    <row r="13" spans="1:26" s="6" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="5" t="s">
-        <v>79</v>
+    <row r="13" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A13" s="2" t="s">
+        <v>76</v>
       </c>
-      <c r="B13" s="2" t="s">
+      <c r="B13" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="F13" s="1"/>
+      <c r="G13" s="9"/>
+      <c r="H13" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="I13" s="1"/>
+      <c r="J13" s="1"/>
+      <c r="K13" s="1"/>
+      <c r="L13" s="1"/>
+      <c r="M13" s="1"/>
+      <c r="N13" s="1"/>
+      <c r="O13" s="1"/>
+      <c r="P13" s="1"/>
+      <c r="Q13" s="1"/>
+      <c r="R13" s="1"/>
+      <c r="S13" s="1"/>
+      <c r="T13" s="1"/>
+      <c r="U13" s="1"/>
+      <c r="V13" s="1"/>
+      <c r="W13" s="1"/>
+      <c r="X13" s="1"/>
+      <c r="Y13" s="1"/>
+      <c r="Z13" s="1"/>
+    </row>
+    <row r="14" spans="1:26" s="6" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="F14" s="5"/>
+      <c r="G14" s="10" t="s">
         <v>74</v>
       </c>
-      <c r="C13" s="2" t="s">
+      <c r="H14" s="5" t="s">
         <v>75</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="E13" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="F13" s="5"/>
-      <c r="G13" s="10" t="s">
-        <v>77</v>
-      </c>
-      <c r="H13" s="5" t="s">
-        <v>78</v>
-      </c>
-      <c r="I13" s="5"/>
-      <c r="J13" s="5"/>
-      <c r="K13" s="5"/>
-      <c r="L13" s="5"/>
-      <c r="M13" s="5"/>
-      <c r="N13" s="5"/>
-      <c r="O13" s="5"/>
-      <c r="P13" s="5"/>
-      <c r="Q13" s="5"/>
-      <c r="R13" s="5"/>
-      <c r="S13" s="5"/>
-      <c r="T13" s="5"/>
-      <c r="U13" s="5"/>
-      <c r="V13" s="5"/>
-      <c r="W13" s="5"/>
-      <c r="X13" s="5"/>
-      <c r="Y13" s="5"/>
-      <c r="Z13" s="5"/>
-    </row>
-    <row r="14" spans="1:26" s="7" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="5" t="s">
-        <v>83</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="D14" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="E14" s="5" t="s">
-        <v>89</v>
-      </c>
-      <c r="F14" s="5"/>
-      <c r="G14" s="10"/>
-      <c r="H14" s="5" t="s">
-        <v>90</v>
       </c>
       <c r="I14" s="5"/>
       <c r="J14" s="5"/>
@@ -2447,28 +2678,26 @@
       <c r="Y14" s="5"/>
       <c r="Z14" s="5"/>
     </row>
-    <row r="15" spans="1:26" s="6" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="5" t="s">
-        <v>92</v>
+    <row r="15" spans="1:26" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="2" t="s">
+        <v>88</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="E15" s="5" t="s">
-        <v>51</v>
+        <v>85</v>
       </c>
       <c r="F15" s="5"/>
-      <c r="G15" s="10" t="s">
-        <v>85</v>
-      </c>
+      <c r="G15" s="10"/>
       <c r="H15" s="5" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="I15" s="5"/>
       <c r="J15" s="5"/>
@@ -2490,14 +2719,28 @@
       <c r="Z15" s="5"/>
     </row>
     <row r="16" spans="1:26" s="6" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="5"/>
-      <c r="B16" s="5"/>
-      <c r="C16" s="5"/>
-      <c r="D16" s="5"/>
-      <c r="E16" s="5"/>
+      <c r="A16" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="E16" s="5" t="s">
+        <v>49</v>
+      </c>
       <c r="F16" s="5"/>
-      <c r="G16" s="10"/>
-      <c r="H16" s="5"/>
+      <c r="G16" s="10" t="s">
+        <v>82</v>
+      </c>
+      <c r="H16" s="5" t="s">
+        <v>87</v>
+      </c>
       <c r="I16" s="5"/>
       <c r="J16" s="5"/>
       <c r="K16" s="5"/>
@@ -2518,42 +2761,65 @@
       <c r="Z16" s="5"/>
     </row>
     <row r="17" spans="1:26" s="6" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="5"/>
-      <c r="B17" s="5"/>
-      <c r="C17" s="5"/>
-      <c r="D17" s="5"/>
-      <c r="E17" s="5"/>
-      <c r="F17" s="5"/>
-      <c r="G17" s="10"/>
-      <c r="H17" s="5"/>
-      <c r="I17" s="5"/>
-      <c r="J17" s="5"/>
-      <c r="K17" s="5"/>
-      <c r="L17" s="5"/>
-      <c r="M17" s="5"/>
-      <c r="N17" s="5"/>
-      <c r="O17" s="5"/>
-      <c r="P17" s="5"/>
-      <c r="Q17" s="5"/>
-      <c r="R17" s="5"/>
-      <c r="S17" s="5"/>
-      <c r="T17" s="5"/>
-      <c r="U17" s="5"/>
-      <c r="V17" s="5"/>
-      <c r="W17" s="5"/>
-      <c r="X17" s="5"/>
-      <c r="Y17" s="5"/>
-      <c r="Z17" s="5"/>
+      <c r="A17" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="D17" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="E17" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="F17" s="1"/>
+      <c r="H17" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="I17" s="1"/>
+      <c r="J17" s="1"/>
+      <c r="K17" s="1"/>
+      <c r="L17" s="1"/>
+      <c r="M17" s="1"/>
+      <c r="N17" s="1"/>
+      <c r="O17" s="1"/>
+      <c r="P17" s="1"/>
+      <c r="Q17" s="1"/>
+      <c r="R17" s="1"/>
+      <c r="S17" s="1"/>
+      <c r="T17" s="1"/>
+      <c r="U17" s="1"/>
+      <c r="V17" s="1"/>
+      <c r="W17" s="1"/>
+      <c r="X17" s="1"/>
+      <c r="Y17" s="1"/>
+      <c r="Z17" s="1"/>
     </row>
     <row r="18" spans="1:26" s="6" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="8"/>
-      <c r="B18" s="8"/>
-      <c r="C18" s="8"/>
-      <c r="D18" s="8"/>
-      <c r="E18" s="8"/>
-      <c r="F18" s="8"/>
+      <c r="A18" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="D18" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="E18" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="F18" s="5"/>
       <c r="G18" s="10"/>
-      <c r="H18" s="5"/>
+      <c r="H18" s="5" t="s">
+        <v>98</v>
+      </c>
       <c r="I18" s="5"/>
       <c r="J18" s="5"/>
       <c r="K18" s="5"/>
@@ -2573,33 +2839,33 @@
       <c r="Y18" s="5"/>
       <c r="Z18" s="5"/>
     </row>
-    <row r="19" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A19" s="4"/>
-      <c r="B19" s="4"/>
-      <c r="C19" s="4"/>
-      <c r="D19" s="4"/>
-      <c r="E19" s="4"/>
-      <c r="F19" s="4"/>
-      <c r="G19" s="9"/>
-      <c r="H19" s="1"/>
-      <c r="I19" s="1"/>
-      <c r="J19" s="1"/>
-      <c r="K19" s="1"/>
-      <c r="L19" s="1"/>
-      <c r="M19" s="1"/>
-      <c r="N19" s="1"/>
-      <c r="O19" s="1"/>
-      <c r="P19" s="1"/>
-      <c r="Q19" s="1"/>
-      <c r="R19" s="1"/>
-      <c r="S19" s="1"/>
-      <c r="T19" s="1"/>
-      <c r="U19" s="1"/>
-      <c r="V19" s="1"/>
-      <c r="W19" s="1"/>
-      <c r="X19" s="1"/>
-      <c r="Y19" s="1"/>
-      <c r="Z19" s="1"/>
+    <row r="19" spans="1:26" s="6" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="8"/>
+      <c r="B19" s="8"/>
+      <c r="C19" s="8"/>
+      <c r="D19" s="8"/>
+      <c r="E19" s="8"/>
+      <c r="F19" s="8"/>
+      <c r="G19" s="10"/>
+      <c r="H19" s="5"/>
+      <c r="I19" s="5"/>
+      <c r="J19" s="5"/>
+      <c r="K19" s="5"/>
+      <c r="L19" s="5"/>
+      <c r="M19" s="5"/>
+      <c r="N19" s="5"/>
+      <c r="O19" s="5"/>
+      <c r="P19" s="5"/>
+      <c r="Q19" s="5"/>
+      <c r="R19" s="5"/>
+      <c r="S19" s="5"/>
+      <c r="T19" s="5"/>
+      <c r="U19" s="5"/>
+      <c r="V19" s="5"/>
+      <c r="W19" s="5"/>
+      <c r="X19" s="5"/>
+      <c r="Y19" s="5"/>
+      <c r="Z19" s="5"/>
     </row>
     <row r="20" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A20" s="4"/>
@@ -2635,7 +2901,7 @@
       <c r="C21" s="4"/>
       <c r="D21" s="4"/>
       <c r="E21" s="4"/>
-      <c r="F21" s="1"/>
+      <c r="F21" s="4"/>
       <c r="G21" s="9"/>
       <c r="H21" s="1"/>
       <c r="I21" s="1"/>
@@ -2658,11 +2924,11 @@
       <c r="Z21" s="1"/>
     </row>
     <row r="22" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A22" s="1"/>
-      <c r="B22" s="1"/>
+      <c r="A22" s="4"/>
+      <c r="B22" s="4"/>
       <c r="C22" s="4"/>
-      <c r="D22" s="1"/>
-      <c r="E22" s="1"/>
+      <c r="D22" s="4"/>
+      <c r="E22" s="4"/>
       <c r="F22" s="1"/>
       <c r="G22" s="9"/>
       <c r="H22" s="1"/>
@@ -2688,7 +2954,7 @@
     <row r="23" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A23" s="1"/>
       <c r="B23" s="1"/>
-      <c r="C23" s="1"/>
+      <c r="C23" s="4"/>
       <c r="D23" s="1"/>
       <c r="E23" s="1"/>
       <c r="F23" s="1"/>
@@ -2773,8 +3039,8 @@
       <c r="A26" s="1"/>
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
-      <c r="D26" s="2"/>
-      <c r="E26" s="2"/>
+      <c r="D26" s="1"/>
+      <c r="E26" s="1"/>
       <c r="F26" s="1"/>
       <c r="G26" s="9"/>
       <c r="H26" s="1"/>
@@ -2801,8 +3067,8 @@
       <c r="A27" s="1"/>
       <c r="B27" s="1"/>
       <c r="C27" s="1"/>
-      <c r="D27" s="1"/>
-      <c r="E27" s="1"/>
+      <c r="D27" s="2"/>
+      <c r="E27" s="2"/>
       <c r="F27" s="1"/>
       <c r="G27" s="9"/>
       <c r="H27" s="1"/>
@@ -30097,6 +30363,34 @@
       <c r="Y1001" s="1"/>
       <c r="Z1001" s="1"/>
     </row>
+    <row r="1002" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A1002" s="1"/>
+      <c r="B1002" s="1"/>
+      <c r="C1002" s="1"/>
+      <c r="D1002" s="1"/>
+      <c r="E1002" s="1"/>
+      <c r="F1002" s="1"/>
+      <c r="G1002" s="9"/>
+      <c r="H1002" s="1"/>
+      <c r="I1002" s="1"/>
+      <c r="J1002" s="1"/>
+      <c r="K1002" s="1"/>
+      <c r="L1002" s="1"/>
+      <c r="M1002" s="1"/>
+      <c r="N1002" s="1"/>
+      <c r="O1002" s="1"/>
+      <c r="P1002" s="1"/>
+      <c r="Q1002" s="1"/>
+      <c r="R1002" s="1"/>
+      <c r="S1002" s="1"/>
+      <c r="T1002" s="1"/>
+      <c r="U1002" s="1"/>
+      <c r="V1002" s="1"/>
+      <c r="W1002" s="1"/>
+      <c r="X1002" s="1"/>
+      <c r="Y1002" s="1"/>
+      <c r="Z1002" s="1"/>
+    </row>
   </sheetData>
   <phoneticPr fontId="23" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>